<commit_message>
added feature to other columns
</commit_message>
<xml_diff>
--- a/data_test.xlsx
+++ b/data_test.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\contact_cleaner\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11235"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="data_test" sheetId="1" r:id="rId4"/>
+    <sheet name="data_test" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
   <si>
     <t>email</t>
   </si>
@@ -40,12 +48,6 @@
     <t>lgpd</t>
   </si>
   <si>
-    <t>teste@1f5.com</t>
-  </si>
-  <si>
-    <t>fulano de teste</t>
-  </si>
-  <si>
     <t>Botafogo</t>
   </si>
   <si>
@@ -61,27 +63,12 @@
     <t>Sim</t>
   </si>
   <si>
-    <t>teste_2@1f5.com</t>
-  </si>
-  <si>
-    <t>sicrano de teste</t>
-  </si>
-  <si>
     <t>Flamengo</t>
   </si>
   <si>
-    <t>Maconha</t>
-  </si>
-  <si>
     <t>muitos bla bla</t>
   </si>
   <si>
-    <t>teste_3@1f5.com</t>
-  </si>
-  <si>
-    <t>cateto de teste</t>
-  </si>
-  <si>
     <t>Centro</t>
   </si>
   <si>
@@ -91,43 +78,92 @@
     <t>MGJd, csd, d</t>
   </si>
   <si>
-    <t>Tijuca</t>
-  </si>
-  <si>
-    <t>Zona Norte</t>
-  </si>
-  <si>
-    <t>teste</t>
-  </si>
-  <si>
-    <t>Não</t>
-  </si>
-  <si>
-    <t>TESTENono@dg.com</t>
-  </si>
-  <si>
-    <t>Paulo de teste</t>
-  </si>
-  <si>
-    <t>Pavuna</t>
+    <t>matriz</t>
+  </si>
+  <si>
+    <t>20-04-2023_teste_form</t>
+  </si>
+  <si>
+    <t>20-04-2023_outro_form</t>
+  </si>
+  <si>
+    <t>GabRiel Souza</t>
+  </si>
+  <si>
+    <t>Leme</t>
+  </si>
+  <si>
+    <t>outras coisas</t>
+  </si>
+  <si>
+    <t>fulano@teste.com</t>
+  </si>
+  <si>
+    <t>sicrano@test.com</t>
+  </si>
+  <si>
+    <t>cateto@test.com</t>
+  </si>
+  <si>
+    <t>fulano teste</t>
+  </si>
+  <si>
+    <t>CATETO TESTE</t>
+  </si>
+  <si>
+    <t>Síçraño téstê</t>
+  </si>
+  <si>
+    <t>fulano teste repetido</t>
+  </si>
+  <si>
+    <t>fulano teste diferent cel</t>
+  </si>
+  <si>
+    <t>fulano teste diferent interesse</t>
+  </si>
+  <si>
+    <t>Saude</t>
+  </si>
+  <si>
+    <t>fulano teste diferent email</t>
+  </si>
+  <si>
+    <t>fulano_diferente@teste.com</t>
+  </si>
+  <si>
+    <t>Gag@email.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-  </numFmts>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -137,39 +173,49 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -359,23 +405,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="8" max="8" width="14.13"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -403,150 +457,281 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="1">
+        <v>999888777</v>
+      </c>
+      <c r="D2" s="2">
+        <v>44999</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1">
-        <v>9.99888777E8</v>
-      </c>
-      <c r="D2" s="2">
-        <v>44999.0</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="1">
+        <v>666555444</v>
+      </c>
+      <c r="D3" s="2">
+        <v>44999</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="I3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1246885</v>
+      </c>
+      <c r="D4" s="2">
+        <v>44999</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="1">
-        <v>6.66555444E8</v>
-      </c>
-      <c r="D3" s="2">
-        <v>44999.0</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="I4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1">
+        <v>999888444</v>
+      </c>
+      <c r="D5" s="5">
+        <v>45036</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="1">
-        <v>3.33222111E8</v>
-      </c>
-      <c r="D4" s="2">
-        <v>44999.0</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="1" t="s">
+    </row>
+    <row r="6" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1">
-        <v>9.99888777E8</v>
-      </c>
-      <c r="D5" s="2">
-        <v>44999.0</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C6" s="1">
-        <v>2.1111222333E10</v>
+        <v>999888777</v>
       </c>
       <c r="D6" s="2">
-        <v>44999.0</v>
+        <v>44999</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="C7" s="1">
+        <v>999888666</v>
+      </c>
+      <c r="D7" s="2">
+        <v>44999</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="J7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="1">
+        <v>999888666</v>
+      </c>
+      <c r="D8" s="2">
+        <v>44999</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="1">
+        <v>999888666</v>
+      </c>
+      <c r="D9" s="2">
+        <v>44999</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E16" s="3"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink ref="A5" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+    <hyperlink ref="A9" r:id="rId8"/>
+  </hyperlinks>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>